<commit_message>
#9790 & #9732 &#9635
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QSI002.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QSI002.xlsx
@@ -285,27 +285,6 @@
     <t>（変更後）</t>
   </si>
   <si>
-    <r>
-      <t>㋒</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐ明朝"/>
-        <family val="1"/>
-        <charset val="128"/>
-      </rPr>
-      <t>　備　考</t>
-    </r>
-    <rPh sb="2" eb="3">
-      <t>ソナエ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>コウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>②　被保険者整理番号</t>
     <rPh sb="2" eb="6">
       <t>ヒホケンシャ</t>
@@ -343,7 +322,7 @@
   </si>
   <si>
     <t>㊞</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>④　 生　　年　　月　　日</t>
@@ -430,7 +409,7 @@
     <rPh sb="2" eb="3">
       <t>とう</t>
     </rPh>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>社会保険労務士記載欄</t>
@@ -506,12 +485,15 @@
   <si>
     <t>　（   　　   　  　局）　</t>
   </si>
+  <si>
+    <t>㋒　備　考</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="32">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -525,79 +507,10 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="ＭＳ 明朝"/>
-      <family val="1"/>
       <charset val="128"/>
     </font>
     <font>
@@ -608,82 +521,9 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="16"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="MS Mincho"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="MS Mincho"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="MS Mincho"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="MS Mincho"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <family val="1"/>
       <charset val="128"/>
     </font>
     <font>
@@ -715,8 +555,75 @@
     </font>
     <font>
       <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
       <sz val="16"/>
-      <name val="ＭＳ Ｐ明朝"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1395,101 +1302,454 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="263">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1499,627 +1759,244 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2158,7 +2035,7 @@
         <xdr:cNvPr id="1605" name="Line 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045060000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000045060000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2217,7 +2094,7 @@
         <xdr:cNvPr id="1606" name="Line 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046060000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000046060000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2276,7 +2153,7 @@
         <xdr:cNvPr id="1608" name="Line 111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048060000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000048060000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2335,7 +2212,7 @@
         <xdr:cNvPr id="1612" name="Group 125">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C060000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004C060000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2346,7 +2223,7 @@
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
           <a:off x="10598426" y="1980786"/>
-          <a:ext cx="171450" cy="1145899"/>
+          <a:ext cx="171450" cy="1096203"/>
           <a:chOff x="1973" y="1410"/>
           <a:chExt cx="272" cy="705"/>
         </a:xfrm>
@@ -2356,7 +2233,7 @@
           <xdr:cNvPr id="1621" name="Oval 126">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055060000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000055060000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2397,7 +2274,7 @@
           <xdr:cNvPr id="1622" name="Oval 127">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056060000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000056060000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2438,7 +2315,7 @@
           <xdr:cNvPr id="1623" name="Rectangle 128">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057060000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000057060000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2495,7 +2372,7 @@
         <xdr:cNvPr id="1154" name="Text Box 130">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000082040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2608,7 +2485,7 @@
         <xdr:cNvPr id="28" name="Text Box 129">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2712,7 +2589,7 @@
         <xdr:cNvPr id="1615" name="Group 135">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F060000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004F060000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2722,8 +2599,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9731237" y="3344103"/>
-          <a:ext cx="152400" cy="894936"/>
+          <a:off x="9731237" y="3294408"/>
+          <a:ext cx="152400" cy="894935"/>
           <a:chOff x="1973" y="1410"/>
           <a:chExt cx="272" cy="705"/>
         </a:xfrm>
@@ -2733,7 +2610,7 @@
           <xdr:cNvPr id="1618" name="Oval 136">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052060000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000052060000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2774,7 +2651,7 @@
           <xdr:cNvPr id="1619" name="Oval 137">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053060000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053060000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2815,7 +2692,7 @@
           <xdr:cNvPr id="1620" name="Rectangle 138">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054060000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000054060000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2872,7 +2749,7 @@
         <xdr:cNvPr id="33" name="Text Box 139">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2985,7 +2862,7 @@
         <xdr:cNvPr id="27" name="テキスト ボックス 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3050,7 +2927,7 @@
         <xdr:cNvPr id="32" name="Line 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3109,7 +2986,7 @@
         <xdr:cNvPr id="21" name="A1_4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3175,7 +3052,7 @@
         <xdr:cNvPr id="22" name="A1_6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3241,7 +3118,7 @@
         <xdr:cNvPr id="23" name="A1_5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3307,7 +3184,7 @@
         <xdr:cNvPr id="24" name="A1_7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3373,7 +3250,7 @@
         <xdr:cNvPr id="26" name="A1_8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3439,7 +3316,7 @@
         <xdr:cNvPr id="29" name="C1_9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3505,7 +3382,7 @@
         <xdr:cNvPr id="31" name="C1_10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3571,7 +3448,7 @@
         <xdr:cNvPr id="34" name="C1_11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3637,7 +3514,7 @@
         <xdr:cNvPr id="35" name="C1_12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3703,7 +3580,7 @@
         <xdr:cNvPr id="36" name="C1_13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3769,7 +3646,7 @@
         <xdr:cNvPr id="37" name="C1_14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3835,7 +3712,7 @@
         <xdr:cNvPr id="42" name="図 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBDBE897-C3CA-49F3-B3BD-41959751EF73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBDBE897-C3CA-49F3-B3BD-41959751EF73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3896,7 +3773,7 @@
         <xdr:cNvPr id="43" name="Picture 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E92B99-4293-4E41-A824-FAD99FACFBA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{10E92B99-4293-4E41-A824-FAD99FACFBA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4268,1389 +4145,1450 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AM37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F10" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="AH18" sqref="AH18:AJ19"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="3.25" style="1" customWidth="1"/>
-    <col min="5" max="10" width="3.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="3.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.125" style="1" customWidth="1"/>
-    <col min="14" max="19" width="3.625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="3.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="3.375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="3.25" style="1" customWidth="1"/>
-    <col min="23" max="24" width="3.125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="3.5" style="1" customWidth="1"/>
-    <col min="26" max="26" width="3.625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="3.75" style="1" customWidth="1"/>
-    <col min="28" max="28" width="3.875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="3.75" style="1" customWidth="1"/>
-    <col min="30" max="30" width="4" style="1" customWidth="1"/>
-    <col min="31" max="31" width="3.875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="3.75" style="1" customWidth="1"/>
-    <col min="33" max="33" width="3.625" style="1" customWidth="1"/>
-    <col min="34" max="35" width="4" style="1" customWidth="1"/>
-    <col min="36" max="36" width="3.25" style="1" customWidth="1"/>
-    <col min="37" max="37" width="1.875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="4.375" style="1" customWidth="1"/>
-    <col min="39" max="39" width="0.125" style="1" customWidth="1"/>
-    <col min="40" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="2.875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="3.375" style="15" customWidth="1"/>
+    <col min="3" max="4" width="3.25" style="15" customWidth="1"/>
+    <col min="5" max="10" width="3.625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="3.875" style="15" customWidth="1"/>
+    <col min="12" max="12" width="11.375" style="15" customWidth="1"/>
+    <col min="13" max="13" width="9.125" style="15" customWidth="1"/>
+    <col min="14" max="19" width="3.625" style="15" customWidth="1"/>
+    <col min="20" max="20" width="3.5" style="15" customWidth="1"/>
+    <col min="21" max="21" width="3.375" style="15" customWidth="1"/>
+    <col min="22" max="22" width="3.25" style="15" customWidth="1"/>
+    <col min="23" max="24" width="3.125" style="15" customWidth="1"/>
+    <col min="25" max="25" width="3.5" style="15" customWidth="1"/>
+    <col min="26" max="26" width="3.625" style="15" customWidth="1"/>
+    <col min="27" max="27" width="3.75" style="15" customWidth="1"/>
+    <col min="28" max="28" width="3.875" style="15" customWidth="1"/>
+    <col min="29" max="29" width="3.75" style="15" customWidth="1"/>
+    <col min="30" max="30" width="4" style="15" customWidth="1"/>
+    <col min="31" max="31" width="3.875" style="15" customWidth="1"/>
+    <col min="32" max="32" width="3.75" style="15" customWidth="1"/>
+    <col min="33" max="33" width="3.625" style="15" customWidth="1"/>
+    <col min="34" max="35" width="4" style="15" customWidth="1"/>
+    <col min="36" max="36" width="3.25" style="15" customWidth="1"/>
+    <col min="37" max="37" width="1.875" style="15" customWidth="1"/>
+    <col min="38" max="38" width="4.375" style="15" customWidth="1"/>
+    <col min="39" max="39" width="0.125" style="15" customWidth="1"/>
+    <col min="40" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="12.75" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
     </row>
     <row r="2" spans="1:39" ht="19.5" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
     </row>
     <row r="3" spans="1:39" ht="9.9499999999999993" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="159" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="160"/>
-      <c r="AA3" s="161"/>
-      <c r="AB3" s="159" t="s">
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="160"/>
-      <c r="AD3" s="161"/>
-      <c r="AE3" s="159" t="s">
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="160"/>
-      <c r="AG3" s="161"/>
-      <c r="AH3" s="159" t="s">
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AI3" s="160"/>
-      <c r="AJ3" s="161"/>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="15"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="26"/>
+      <c r="AL3" s="27"/>
     </row>
     <row r="4" spans="1:39" ht="9.9499999999999993" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="156" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="Z4" s="157"/>
-      <c r="AA4" s="158"/>
-      <c r="AB4" s="156" t="s">
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="AC4" s="157"/>
-      <c r="AD4" s="158"/>
-      <c r="AE4" s="156" t="s">
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AF4" s="157"/>
-      <c r="AG4" s="158"/>
-      <c r="AH4" s="156"/>
-      <c r="AI4" s="157"/>
-      <c r="AJ4" s="158"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="15"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="30"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="27"/>
     </row>
     <row r="5" spans="1:39" ht="26.25" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="103" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="118" t="s">
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="118"/>
-      <c r="R5" s="118"/>
-      <c r="S5" s="118"/>
-      <c r="T5" s="118"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="144"/>
-      <c r="Z5" s="145"/>
-      <c r="AA5" s="146"/>
-      <c r="AB5" s="144"/>
-      <c r="AC5" s="145"/>
-      <c r="AD5" s="146"/>
-      <c r="AE5" s="144"/>
-      <c r="AF5" s="145"/>
-      <c r="AG5" s="146"/>
-      <c r="AH5" s="144"/>
-      <c r="AI5" s="145"/>
-      <c r="AJ5" s="146"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="139"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="33"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="32"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="34"/>
+      <c r="AH5" s="32"/>
+      <c r="AI5" s="33"/>
+      <c r="AJ5" s="34"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="36"/>
     </row>
     <row r="6" spans="1:39" ht="27.75" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="155" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="155"/>
-      <c r="L6" s="155"/>
-      <c r="M6" s="118"/>
-      <c r="N6" s="118"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="118"/>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
-      <c r="S6" s="118"/>
-      <c r="T6" s="118"/>
-      <c r="U6" s="118"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="147"/>
-      <c r="Z6" s="148"/>
-      <c r="AA6" s="149"/>
-      <c r="AB6" s="147"/>
-      <c r="AC6" s="148"/>
-      <c r="AD6" s="149"/>
-      <c r="AE6" s="147"/>
-      <c r="AF6" s="148"/>
-      <c r="AG6" s="149"/>
-      <c r="AH6" s="147"/>
-      <c r="AI6" s="148"/>
-      <c r="AJ6" s="149"/>
-      <c r="AK6" s="6"/>
-      <c r="AL6" s="139"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="40"/>
+      <c r="AH6" s="38"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="40"/>
+      <c r="AK6" s="35"/>
+      <c r="AL6" s="36"/>
     </row>
     <row r="7" spans="1:39" ht="35.25" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="14"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="14"/>
     </row>
     <row r="8" spans="1:39" ht="13.5" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="102" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="144" t="s">
+      <c r="E8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="33"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="145"/>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="146"/>
-      <c r="K8" s="144" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="145"/>
-      <c r="M8" s="146"/>
-      <c r="N8" s="144" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="145"/>
-      <c r="P8" s="145"/>
-      <c r="Q8" s="145"/>
-      <c r="R8" s="145"/>
-      <c r="S8" s="145"/>
-      <c r="T8" s="145"/>
-      <c r="U8" s="145"/>
-      <c r="V8" s="145"/>
-      <c r="W8" s="145"/>
-      <c r="X8" s="145"/>
-      <c r="Y8" s="146"/>
-      <c r="Z8" s="144" t="s">
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA8" s="33"/>
+      <c r="AB8" s="33"/>
+      <c r="AC8" s="33"/>
+      <c r="AD8" s="33"/>
+      <c r="AE8" s="33"/>
+      <c r="AF8" s="33"/>
+      <c r="AG8" s="34"/>
+      <c r="AH8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="145"/>
-      <c r="AC8" s="145"/>
-      <c r="AD8" s="145"/>
-      <c r="AE8" s="145"/>
-      <c r="AF8" s="145"/>
-      <c r="AG8" s="146"/>
-      <c r="AH8" s="150" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI8" s="151"/>
-      <c r="AJ8" s="221"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="12"/>
+      <c r="AI8" s="44"/>
+      <c r="AJ8" s="45"/>
+      <c r="AK8" s="46"/>
+      <c r="AL8" s="47"/>
     </row>
     <row r="9" spans="1:39">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="111"/>
-      <c r="N9" s="109"/>
-      <c r="O9" s="110"/>
-      <c r="P9" s="110"/>
-      <c r="Q9" s="110"/>
-      <c r="R9" s="110"/>
-      <c r="S9" s="110"/>
-      <c r="T9" s="110"/>
-      <c r="U9" s="110"/>
-      <c r="V9" s="110"/>
-      <c r="W9" s="110"/>
-      <c r="X9" s="110"/>
-      <c r="Y9" s="111"/>
-      <c r="Z9" s="109"/>
-      <c r="AA9" s="110"/>
-      <c r="AB9" s="110"/>
-      <c r="AC9" s="110"/>
-      <c r="AD9" s="110"/>
-      <c r="AE9" s="110"/>
-      <c r="AF9" s="110"/>
-      <c r="AG9" s="111"/>
-      <c r="AH9" s="140" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI9" s="141"/>
-      <c r="AJ9" s="222"/>
-      <c r="AK9" s="8"/>
-      <c r="AL9" s="12"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="50"/>
+      <c r="Z9" s="48"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="49"/>
+      <c r="AG9" s="50"/>
+      <c r="AH9" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI9" s="52"/>
+      <c r="AJ9" s="53"/>
+      <c r="AK9" s="46"/>
+      <c r="AL9" s="47"/>
     </row>
-    <row r="10" spans="1:39" ht="16.5" thickBot="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="152"/>
-      <c r="L10" s="153"/>
-      <c r="M10" s="154"/>
-      <c r="N10" s="152"/>
-      <c r="O10" s="153"/>
-      <c r="P10" s="153"/>
-      <c r="Q10" s="153"/>
-      <c r="R10" s="153"/>
-      <c r="S10" s="153"/>
-      <c r="T10" s="153"/>
-      <c r="U10" s="153"/>
-      <c r="V10" s="153"/>
-      <c r="W10" s="153"/>
-      <c r="X10" s="153"/>
-      <c r="Y10" s="154"/>
-      <c r="Z10" s="152"/>
-      <c r="AA10" s="153"/>
-      <c r="AB10" s="153"/>
-      <c r="AC10" s="153"/>
-      <c r="AD10" s="153"/>
-      <c r="AE10" s="153"/>
-      <c r="AF10" s="153"/>
-      <c r="AG10" s="154"/>
-      <c r="AH10" s="142" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI10" s="143"/>
-      <c r="AJ10" s="222"/>
-      <c r="AK10" s="8"/>
-      <c r="AL10" s="12"/>
+    <row r="10" spans="1:39" ht="14.25" thickBot="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
+      <c r="V10" s="55"/>
+      <c r="W10" s="55"/>
+      <c r="X10" s="55"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="55"/>
+      <c r="AC10" s="55"/>
+      <c r="AD10" s="55"/>
+      <c r="AE10" s="55"/>
+      <c r="AF10" s="55"/>
+      <c r="AG10" s="56"/>
+      <c r="AH10" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI10" s="58"/>
+      <c r="AJ10" s="53"/>
+      <c r="AK10" s="46"/>
+      <c r="AL10" s="47"/>
     </row>
     <row r="11" spans="1:39" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="184"/>
-      <c r="L11" s="185"/>
-      <c r="M11" s="186"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="207" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA11" s="208"/>
-      <c r="AB11" s="35"/>
-      <c r="AC11" s="35" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68"/>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="68"/>
+      <c r="U11" s="68"/>
+      <c r="V11" s="68"/>
+      <c r="W11" s="68"/>
+      <c r="X11" s="68"/>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA11" s="71"/>
+      <c r="AB11" s="72"/>
+      <c r="AC11" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD11" s="72"/>
+      <c r="AE11" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="AD11" s="35"/>
-      <c r="AE11" s="35" t="s">
+      <c r="AF11" s="72"/>
+      <c r="AG11" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="AF11" s="35"/>
-      <c r="AG11" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH11" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI11" s="18"/>
-      <c r="AJ11" s="222"/>
-      <c r="AK11" s="8"/>
-      <c r="AL11" s="12"/>
+      <c r="AI11" s="75"/>
+      <c r="AJ11" s="53"/>
+      <c r="AK11" s="46"/>
+      <c r="AL11" s="47"/>
     </row>
     <row r="12" spans="1:39" ht="12" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="102"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="178"/>
-      <c r="H12" s="180"/>
-      <c r="I12" s="180"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="187"/>
-      <c r="L12" s="188"/>
-      <c r="M12" s="189"/>
-      <c r="N12" s="104"/>
-      <c r="O12" s="176"/>
-      <c r="P12" s="169"/>
-      <c r="Q12" s="165"/>
-      <c r="R12" s="169"/>
-      <c r="S12" s="176"/>
-      <c r="T12" s="169"/>
-      <c r="U12" s="165"/>
-      <c r="V12" s="169"/>
-      <c r="W12" s="180"/>
-      <c r="X12" s="180"/>
-      <c r="Y12" s="167"/>
-      <c r="Z12" s="209"/>
-      <c r="AA12" s="210"/>
-      <c r="AB12" s="178"/>
-      <c r="AC12" s="193"/>
-      <c r="AD12" s="178"/>
-      <c r="AE12" s="193"/>
-      <c r="AF12" s="178"/>
-      <c r="AG12" s="167"/>
-      <c r="AH12" s="38" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="85"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="85"/>
+      <c r="T12" s="86"/>
+      <c r="U12" s="87"/>
+      <c r="V12" s="86"/>
+      <c r="W12" s="79"/>
+      <c r="X12" s="79"/>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="88"/>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="78"/>
+      <c r="AC12" s="90"/>
+      <c r="AD12" s="78"/>
+      <c r="AE12" s="90"/>
+      <c r="AF12" s="78"/>
+      <c r="AG12" s="80"/>
+      <c r="AH12" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI12" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="AI12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ12" s="222"/>
-      <c r="AK12" s="8"/>
-      <c r="AL12" s="12"/>
+      <c r="AJ12" s="53"/>
+      <c r="AK12" s="46"/>
+      <c r="AL12" s="47"/>
     </row>
     <row r="13" spans="1:39" ht="12" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="178"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="180"/>
-      <c r="J13" s="182"/>
-      <c r="K13" s="187"/>
-      <c r="L13" s="188"/>
-      <c r="M13" s="189"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="176"/>
-      <c r="P13" s="169"/>
-      <c r="Q13" s="165"/>
-      <c r="R13" s="169"/>
-      <c r="S13" s="176"/>
-      <c r="T13" s="169"/>
-      <c r="U13" s="165"/>
-      <c r="V13" s="169"/>
-      <c r="W13" s="180"/>
-      <c r="X13" s="180"/>
-      <c r="Y13" s="167"/>
-      <c r="Z13" s="209"/>
-      <c r="AA13" s="210"/>
-      <c r="AB13" s="178"/>
-      <c r="AC13" s="193"/>
-      <c r="AD13" s="178"/>
-      <c r="AE13" s="193"/>
-      <c r="AF13" s="178"/>
-      <c r="AG13" s="167"/>
-      <c r="AH13" s="38" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="83"/>
+      <c r="N13" s="84"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="86"/>
+      <c r="W13" s="79"/>
+      <c r="X13" s="79"/>
+      <c r="Y13" s="80"/>
+      <c r="Z13" s="88"/>
+      <c r="AA13" s="89"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="90"/>
+      <c r="AD13" s="78"/>
+      <c r="AE13" s="90"/>
+      <c r="AF13" s="78"/>
+      <c r="AG13" s="80"/>
+      <c r="AH13" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI13" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="AI13" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ13" s="222"/>
-      <c r="AK13" s="8"/>
-      <c r="AL13" s="12"/>
+      <c r="AJ13" s="53"/>
+      <c r="AK13" s="46"/>
+      <c r="AL13" s="47"/>
     </row>
     <row r="14" spans="1:39" ht="12" customHeight="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="102"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="116"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="178"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="180"/>
-      <c r="J14" s="182"/>
-      <c r="K14" s="187"/>
-      <c r="L14" s="188"/>
-      <c r="M14" s="189"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="176"/>
-      <c r="P14" s="169"/>
-      <c r="Q14" s="165"/>
-      <c r="R14" s="169"/>
-      <c r="S14" s="176"/>
-      <c r="T14" s="169"/>
-      <c r="U14" s="165"/>
-      <c r="V14" s="169"/>
-      <c r="W14" s="180"/>
-      <c r="X14" s="180"/>
-      <c r="Y14" s="167"/>
-      <c r="Z14" s="209"/>
-      <c r="AA14" s="210"/>
-      <c r="AB14" s="178"/>
-      <c r="AC14" s="193"/>
-      <c r="AD14" s="178"/>
-      <c r="AE14" s="193"/>
-      <c r="AF14" s="178"/>
-      <c r="AG14" s="167"/>
-      <c r="AH14" s="38"/>
-      <c r="AI14" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ14" s="222"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="12"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="83"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="85"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="87"/>
+      <c r="R14" s="86"/>
+      <c r="S14" s="85"/>
+      <c r="T14" s="86"/>
+      <c r="U14" s="87"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="79"/>
+      <c r="X14" s="79"/>
+      <c r="Y14" s="80"/>
+      <c r="Z14" s="88"/>
+      <c r="AA14" s="89"/>
+      <c r="AB14" s="78"/>
+      <c r="AC14" s="90"/>
+      <c r="AD14" s="78"/>
+      <c r="AE14" s="90"/>
+      <c r="AF14" s="78"/>
+      <c r="AG14" s="80"/>
+      <c r="AH14" s="91"/>
+      <c r="AI14" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ14" s="53"/>
+      <c r="AK14" s="46"/>
+      <c r="AL14" s="47"/>
     </row>
     <row r="15" spans="1:39" ht="9" customHeight="1" thickBot="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="179"/>
-      <c r="H15" s="181"/>
-      <c r="I15" s="181"/>
-      <c r="J15" s="183"/>
-      <c r="K15" s="190"/>
-      <c r="L15" s="191"/>
-      <c r="M15" s="192"/>
-      <c r="N15" s="105"/>
-      <c r="O15" s="177"/>
-      <c r="P15" s="170"/>
-      <c r="Q15" s="166"/>
-      <c r="R15" s="170"/>
-      <c r="S15" s="177"/>
-      <c r="T15" s="170"/>
-      <c r="U15" s="166"/>
-      <c r="V15" s="170"/>
-      <c r="W15" s="181"/>
-      <c r="X15" s="181"/>
-      <c r="Y15" s="168"/>
-      <c r="Z15" s="211"/>
-      <c r="AA15" s="212"/>
-      <c r="AB15" s="179"/>
-      <c r="AC15" s="194"/>
-      <c r="AD15" s="179"/>
-      <c r="AE15" s="194"/>
-      <c r="AF15" s="179"/>
-      <c r="AG15" s="168"/>
-      <c r="AH15" s="39"/>
-      <c r="AI15" s="21"/>
-      <c r="AJ15" s="223"/>
-      <c r="AK15" s="8"/>
-      <c r="AL15" s="12"/>
-      <c r="AM15" s="9"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="101"/>
+      <c r="P15" s="102"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="102"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="102"/>
+      <c r="U15" s="103"/>
+      <c r="V15" s="102"/>
+      <c r="W15" s="96"/>
+      <c r="X15" s="96"/>
+      <c r="Y15" s="97"/>
+      <c r="Z15" s="104"/>
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="95"/>
+      <c r="AC15" s="94"/>
+      <c r="AD15" s="95"/>
+      <c r="AE15" s="94"/>
+      <c r="AF15" s="95"/>
+      <c r="AG15" s="97"/>
+      <c r="AH15" s="106"/>
+      <c r="AI15" s="107"/>
+      <c r="AJ15" s="108"/>
+      <c r="AK15" s="46"/>
+      <c r="AL15" s="47"/>
+      <c r="AM15" s="109"/>
     </row>
     <row r="16" spans="1:39" ht="11.25" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="162" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="111"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="137"/>
-      <c r="L16" s="138"/>
-      <c r="M16" s="163" t="s">
+      <c r="K16" s="113"/>
+      <c r="L16" s="114"/>
+      <c r="M16" s="115" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="113"/>
+      <c r="O16" s="113"/>
+      <c r="P16" s="116"/>
+      <c r="Q16" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="N16" s="137"/>
-      <c r="O16" s="137"/>
-      <c r="P16" s="164"/>
-      <c r="Q16" s="171" t="s">
+      <c r="R16" s="118"/>
+      <c r="S16" s="118"/>
+      <c r="T16" s="119"/>
+      <c r="U16" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="R16" s="172"/>
-      <c r="S16" s="172"/>
-      <c r="T16" s="173"/>
-      <c r="U16" s="136" t="s">
-        <v>43</v>
-      </c>
-      <c r="V16" s="137"/>
-      <c r="W16" s="137"/>
-      <c r="X16" s="137"/>
-      <c r="Y16" s="138"/>
-      <c r="Z16" s="244" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA16" s="245"/>
-      <c r="AB16" s="245"/>
-      <c r="AC16" s="246"/>
-      <c r="AD16" s="238" t="s">
+      <c r="V16" s="113"/>
+      <c r="W16" s="113"/>
+      <c r="X16" s="113"/>
+      <c r="Y16" s="114"/>
+      <c r="Z16" s="121" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA16" s="122"/>
+      <c r="AB16" s="122"/>
+      <c r="AC16" s="123"/>
+      <c r="AD16" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="AE16" s="239"/>
-      <c r="AF16" s="239"/>
-      <c r="AG16" s="196"/>
-      <c r="AH16" s="234" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI16" s="234"/>
-      <c r="AJ16" s="235"/>
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="12"/>
-      <c r="AM16" s="9"/>
+      <c r="AE16" s="125"/>
+      <c r="AF16" s="125"/>
+      <c r="AG16" s="126"/>
+      <c r="AH16" s="127" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI16" s="127"/>
+      <c r="AJ16" s="128"/>
+      <c r="AK16" s="46"/>
+      <c r="AL16" s="47"/>
+      <c r="AM16" s="109"/>
     </row>
     <row r="17" spans="1:39" ht="27.75" customHeight="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="102"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="125"/>
-      <c r="K17" s="126"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="122"/>
-      <c r="N17" s="123"/>
-      <c r="O17" s="123"/>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="174"/>
-      <c r="R17" s="110"/>
-      <c r="S17" s="110"/>
-      <c r="T17" s="111"/>
-      <c r="U17" s="203"/>
-      <c r="V17" s="188"/>
-      <c r="W17" s="188"/>
-      <c r="X17" s="188"/>
-      <c r="Y17" s="204"/>
-      <c r="Z17" s="198"/>
-      <c r="AA17" s="188"/>
-      <c r="AB17" s="188"/>
-      <c r="AC17" s="199"/>
-      <c r="AD17" s="240"/>
-      <c r="AE17" s="241"/>
-      <c r="AF17" s="241"/>
-      <c r="AG17" s="197"/>
-      <c r="AH17" s="236"/>
-      <c r="AI17" s="236"/>
-      <c r="AJ17" s="237"/>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="12"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="129" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="130"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="130"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="132"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="133"/>
+      <c r="N17" s="134"/>
+      <c r="O17" s="134"/>
+      <c r="P17" s="135"/>
+      <c r="Q17" s="136"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="137"/>
+      <c r="V17" s="82"/>
+      <c r="W17" s="82"/>
+      <c r="X17" s="82"/>
+      <c r="Y17" s="138"/>
+      <c r="Z17" s="139"/>
+      <c r="AA17" s="82"/>
+      <c r="AB17" s="82"/>
+      <c r="AC17" s="140"/>
+      <c r="AD17" s="141"/>
+      <c r="AE17" s="142"/>
+      <c r="AF17" s="142"/>
+      <c r="AG17" s="143"/>
+      <c r="AH17" s="144"/>
+      <c r="AI17" s="144"/>
+      <c r="AJ17" s="145"/>
+      <c r="AK17" s="146"/>
+      <c r="AL17" s="47"/>
     </row>
     <row r="18" spans="1:39" ht="11.25" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="102"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="131" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="131"/>
-      <c r="H18" s="131"/>
-      <c r="I18" s="132"/>
-      <c r="J18" s="133" t="s">
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="149"/>
+      <c r="J18" s="150" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="151"/>
+      <c r="L18" s="152"/>
+      <c r="M18" s="153"/>
+      <c r="N18" s="154"/>
+      <c r="O18" s="154"/>
+      <c r="P18" s="155"/>
+      <c r="Q18" s="136"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="137"/>
+      <c r="V18" s="82"/>
+      <c r="W18" s="82"/>
+      <c r="X18" s="82"/>
+      <c r="Y18" s="138"/>
+      <c r="Z18" s="139"/>
+      <c r="AA18" s="82"/>
+      <c r="AB18" s="82"/>
+      <c r="AC18" s="140"/>
+      <c r="AD18" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="134"/>
-      <c r="L18" s="135"/>
-      <c r="M18" s="247"/>
-      <c r="N18" s="248"/>
-      <c r="O18" s="248"/>
-      <c r="P18" s="249"/>
-      <c r="Q18" s="174"/>
-      <c r="R18" s="110"/>
-      <c r="S18" s="110"/>
-      <c r="T18" s="111"/>
-      <c r="U18" s="203"/>
-      <c r="V18" s="188"/>
-      <c r="W18" s="188"/>
-      <c r="X18" s="188"/>
-      <c r="Y18" s="204"/>
-      <c r="Z18" s="198"/>
-      <c r="AA18" s="188"/>
-      <c r="AB18" s="188"/>
-      <c r="AC18" s="199"/>
-      <c r="AD18" s="228" t="s">
+      <c r="AE18" s="157" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF18" s="158" t="s">
         <v>46</v>
       </c>
-      <c r="AE18" s="230" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF18" s="242" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG18" s="197"/>
-      <c r="AH18" s="224"/>
-      <c r="AI18" s="224"/>
-      <c r="AJ18" s="225"/>
-      <c r="AK18" s="10"/>
-      <c r="AL18" s="12"/>
+      <c r="AG18" s="143"/>
+      <c r="AH18" s="159"/>
+      <c r="AI18" s="159"/>
+      <c r="AJ18" s="160"/>
+      <c r="AK18" s="146"/>
+      <c r="AL18" s="47"/>
     </row>
     <row r="19" spans="1:39" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="232"/>
-      <c r="K19" s="129"/>
-      <c r="L19" s="233"/>
-      <c r="M19" s="128"/>
-      <c r="N19" s="129"/>
-      <c r="O19" s="129"/>
-      <c r="P19" s="130"/>
-      <c r="Q19" s="175"/>
-      <c r="R19" s="148"/>
-      <c r="S19" s="148"/>
-      <c r="T19" s="149"/>
-      <c r="U19" s="205"/>
-      <c r="V19" s="201"/>
-      <c r="W19" s="201"/>
-      <c r="X19" s="201"/>
-      <c r="Y19" s="206"/>
-      <c r="Z19" s="200"/>
-      <c r="AA19" s="201"/>
-      <c r="AB19" s="201"/>
-      <c r="AC19" s="202"/>
-      <c r="AD19" s="229"/>
-      <c r="AE19" s="231"/>
-      <c r="AF19" s="243"/>
-      <c r="AG19" s="197"/>
-      <c r="AH19" s="226"/>
-      <c r="AI19" s="226"/>
-      <c r="AJ19" s="227"/>
-      <c r="AK19" s="8"/>
-      <c r="AL19" s="12"/>
-      <c r="AM19" s="11"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="161"/>
+      <c r="F19" s="162"/>
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="163"/>
+      <c r="J19" s="164"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="166"/>
+      <c r="M19" s="167"/>
+      <c r="N19" s="165"/>
+      <c r="O19" s="165"/>
+      <c r="P19" s="168"/>
+      <c r="Q19" s="169"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="170"/>
+      <c r="V19" s="171"/>
+      <c r="W19" s="171"/>
+      <c r="X19" s="171"/>
+      <c r="Y19" s="172"/>
+      <c r="Z19" s="173"/>
+      <c r="AA19" s="171"/>
+      <c r="AB19" s="171"/>
+      <c r="AC19" s="174"/>
+      <c r="AD19" s="175"/>
+      <c r="AE19" s="176"/>
+      <c r="AF19" s="177"/>
+      <c r="AG19" s="143"/>
+      <c r="AH19" s="178"/>
+      <c r="AI19" s="178"/>
+      <c r="AJ19" s="179"/>
+      <c r="AK19" s="46"/>
+      <c r="AL19" s="47"/>
+      <c r="AM19" s="180"/>
     </row>
     <row r="20" spans="1:39" ht="33" customHeight="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="102"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="110" t="s">
-        <v>56</v>
-      </c>
-      <c r="V20" s="110"/>
-      <c r="W20" s="82"/>
-      <c r="X20" s="40" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="181"/>
+      <c r="K20" s="181"/>
+      <c r="L20" s="181"/>
+      <c r="M20" s="181"/>
+      <c r="N20" s="181"/>
+      <c r="O20" s="181"/>
+      <c r="P20" s="181"/>
+      <c r="Q20" s="181"/>
+      <c r="R20" s="181"/>
+      <c r="S20" s="181"/>
+      <c r="T20" s="181"/>
+      <c r="U20" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="V20" s="49"/>
+      <c r="W20" s="182"/>
+      <c r="X20" s="183" t="s">
         <v>0</v>
       </c>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="40" t="s">
+      <c r="Y20" s="182"/>
+      <c r="Z20" s="183" t="s">
         <v>1</v>
       </c>
-      <c r="AA20" s="82"/>
-      <c r="AB20" s="41" t="s">
+      <c r="AA20" s="182"/>
+      <c r="AB20" s="184" t="s">
         <v>2</v>
       </c>
-      <c r="AC20" s="40" t="s">
+      <c r="AC20" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="19"/>
-      <c r="AF20" s="19"/>
-      <c r="AG20" s="19"/>
-      <c r="AH20" s="19"/>
-      <c r="AI20" s="19"/>
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="12"/>
-      <c r="AL20" s="12"/>
+      <c r="AD20" s="181"/>
+      <c r="AE20" s="181"/>
+      <c r="AF20" s="181"/>
+      <c r="AG20" s="181"/>
+      <c r="AH20" s="181"/>
+      <c r="AI20" s="181"/>
+      <c r="AJ20" s="181"/>
+      <c r="AK20" s="47"/>
+      <c r="AL20" s="47"/>
     </row>
     <row r="21" spans="1:39" ht="16.899999999999999" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="121"/>
-      <c r="J21" s="213" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="214"/>
-      <c r="L21" s="214"/>
-      <c r="M21" s="214"/>
-      <c r="N21" s="214"/>
-      <c r="O21" s="214"/>
-      <c r="P21" s="214"/>
-      <c r="Q21" s="214"/>
-      <c r="R21" s="214"/>
-      <c r="S21" s="214"/>
-      <c r="T21" s="83"/>
-      <c r="U21" s="83"/>
-      <c r="V21" s="84"/>
-      <c r="W21" s="22"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="19"/>
-      <c r="AF21" s="19"/>
-      <c r="AG21" s="25"/>
-      <c r="AH21" s="195" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="185"/>
+      <c r="F21" s="186"/>
+      <c r="G21" s="186"/>
+      <c r="H21" s="186"/>
+      <c r="I21" s="187"/>
+      <c r="J21" s="188" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="189"/>
+      <c r="L21" s="189"/>
+      <c r="M21" s="189"/>
+      <c r="N21" s="189"/>
+      <c r="O21" s="189"/>
+      <c r="P21" s="189"/>
+      <c r="Q21" s="189"/>
+      <c r="R21" s="189"/>
+      <c r="S21" s="189"/>
+      <c r="T21" s="190"/>
+      <c r="U21" s="190"/>
+      <c r="V21" s="191"/>
+      <c r="W21" s="192"/>
+      <c r="X21" s="193"/>
+      <c r="Y21" s="194"/>
+      <c r="Z21" s="181"/>
+      <c r="AA21" s="181"/>
+      <c r="AB21" s="181"/>
+      <c r="AC21" s="181"/>
+      <c r="AD21" s="181"/>
+      <c r="AE21" s="181"/>
+      <c r="AF21" s="181"/>
+      <c r="AG21" s="195"/>
+      <c r="AH21" s="196" t="s">
         <v>7</v>
       </c>
-      <c r="AI21" s="195"/>
-      <c r="AJ21" s="26"/>
-      <c r="AK21" s="12"/>
-      <c r="AL21" s="12"/>
+      <c r="AI21" s="196"/>
+      <c r="AJ21" s="197"/>
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="47"/>
     </row>
     <row r="22" spans="1:39" ht="16.899999999999999" customHeight="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="250" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="131"/>
-      <c r="G22" s="131"/>
-      <c r="H22" s="131"/>
-      <c r="I22" s="251"/>
-      <c r="J22" s="261" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="198" t="s">
         <v>52</v>
       </c>
-      <c r="K22" s="262"/>
-      <c r="L22" s="262"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
-      <c r="S22" s="46"/>
-      <c r="T22" s="46"/>
-      <c r="U22" s="46"/>
-      <c r="V22" s="85"/>
-      <c r="W22" s="22"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="19"/>
-      <c r="AB22" s="19"/>
-      <c r="AC22" s="19"/>
-      <c r="AD22" s="19"/>
-      <c r="AE22" s="19"/>
-      <c r="AF22" s="19"/>
-      <c r="AG22" s="19"/>
-      <c r="AH22" s="79"/>
-      <c r="AI22" s="79"/>
-      <c r="AJ22" s="80"/>
-      <c r="AK22" s="12"/>
-      <c r="AL22" s="12"/>
+      <c r="F22" s="148"/>
+      <c r="G22" s="148"/>
+      <c r="H22" s="148"/>
+      <c r="I22" s="199"/>
+      <c r="J22" s="200" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="201"/>
+      <c r="L22" s="201"/>
+      <c r="M22" s="130"/>
+      <c r="N22" s="130"/>
+      <c r="O22" s="130"/>
+      <c r="P22" s="130"/>
+      <c r="Q22" s="130"/>
+      <c r="R22" s="130"/>
+      <c r="S22" s="130"/>
+      <c r="T22" s="130"/>
+      <c r="U22" s="130"/>
+      <c r="V22" s="202"/>
+      <c r="W22" s="192"/>
+      <c r="X22" s="193"/>
+      <c r="Y22" s="194"/>
+      <c r="Z22" s="181"/>
+      <c r="AA22" s="181"/>
+      <c r="AB22" s="181"/>
+      <c r="AC22" s="181"/>
+      <c r="AD22" s="181"/>
+      <c r="AE22" s="181"/>
+      <c r="AF22" s="181"/>
+      <c r="AG22" s="181"/>
+      <c r="AH22" s="203"/>
+      <c r="AI22" s="203"/>
+      <c r="AJ22" s="204"/>
+      <c r="AK22" s="47"/>
+      <c r="AL22" s="47"/>
     </row>
     <row r="23" spans="1:39" ht="30" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="102"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="215"/>
-      <c r="L23" s="216"/>
-      <c r="M23" s="216"/>
-      <c r="N23" s="216"/>
-      <c r="O23" s="216"/>
-      <c r="P23" s="216"/>
-      <c r="Q23" s="216"/>
-      <c r="R23" s="216"/>
-      <c r="S23" s="216"/>
-      <c r="T23" s="216"/>
-      <c r="U23" s="77"/>
-      <c r="V23" s="78"/>
-      <c r="W23" s="22"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="19"/>
-      <c r="AH23" s="79"/>
-      <c r="AI23" s="79"/>
-      <c r="AJ23" s="80"/>
-      <c r="AK23" s="12"/>
-      <c r="AL23" s="12"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="206"/>
+      <c r="G23" s="206"/>
+      <c r="H23" s="206"/>
+      <c r="I23" s="207"/>
+      <c r="J23" s="208"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="209"/>
+      <c r="V23" s="210"/>
+      <c r="W23" s="192"/>
+      <c r="X23" s="193"/>
+      <c r="Y23" s="194"/>
+      <c r="Z23" s="181"/>
+      <c r="AA23" s="181"/>
+      <c r="AB23" s="181"/>
+      <c r="AC23" s="181"/>
+      <c r="AD23" s="181"/>
+      <c r="AE23" s="181"/>
+      <c r="AF23" s="181"/>
+      <c r="AG23" s="181"/>
+      <c r="AH23" s="203"/>
+      <c r="AI23" s="203"/>
+      <c r="AJ23" s="204"/>
+      <c r="AK23" s="47"/>
+      <c r="AL23" s="47"/>
     </row>
     <row r="24" spans="1:39" ht="30" customHeight="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="102"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="106" t="s">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="211" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="107"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="108"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="217"/>
-      <c r="L24" s="218"/>
-      <c r="M24" s="218"/>
-      <c r="N24" s="218"/>
-      <c r="O24" s="218"/>
-      <c r="P24" s="218"/>
-      <c r="Q24" s="218"/>
-      <c r="R24" s="218"/>
-      <c r="S24" s="218"/>
-      <c r="T24" s="218"/>
-      <c r="U24" s="70"/>
-      <c r="V24" s="71"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
-      <c r="Z24" s="19"/>
-      <c r="AA24" s="19"/>
-      <c r="AB24" s="19"/>
-      <c r="AC24" s="19"/>
-      <c r="AD24" s="19"/>
-      <c r="AE24" s="19"/>
-      <c r="AF24" s="19"/>
-      <c r="AG24" s="19"/>
-      <c r="AH24" s="19"/>
-      <c r="AI24" s="19"/>
-      <c r="AJ24" s="19"/>
-      <c r="AK24" s="12"/>
-      <c r="AL24" s="12"/>
+      <c r="F24" s="212"/>
+      <c r="G24" s="212"/>
+      <c r="H24" s="212"/>
+      <c r="I24" s="213"/>
+      <c r="J24" s="214"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="215"/>
+      <c r="V24" s="216"/>
+      <c r="W24" s="217"/>
+      <c r="X24" s="194"/>
+      <c r="Y24" s="194"/>
+      <c r="Z24" s="181"/>
+      <c r="AA24" s="181"/>
+      <c r="AB24" s="181"/>
+      <c r="AC24" s="181"/>
+      <c r="AD24" s="181"/>
+      <c r="AE24" s="181"/>
+      <c r="AF24" s="181"/>
+      <c r="AG24" s="181"/>
+      <c r="AH24" s="181"/>
+      <c r="AI24" s="181"/>
+      <c r="AJ24" s="181"/>
+      <c r="AK24" s="47"/>
+      <c r="AL24" s="47"/>
     </row>
     <row r="25" spans="1:39" ht="28.9" customHeight="1">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="109" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="111"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="219"/>
-      <c r="L25" s="220"/>
-      <c r="M25" s="220"/>
-      <c r="N25" s="220"/>
-      <c r="O25" s="220"/>
-      <c r="P25" s="220"/>
-      <c r="Q25" s="220"/>
-      <c r="R25" s="220"/>
-      <c r="S25" s="220"/>
-      <c r="T25" s="81"/>
-      <c r="U25" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="V25" s="19"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="19"/>
-      <c r="AD25" s="19"/>
-      <c r="AE25" s="19"/>
-      <c r="AF25" s="19"/>
-      <c r="AG25" s="19"/>
-      <c r="AH25" s="19"/>
-      <c r="AI25" s="19"/>
-      <c r="AJ25" s="19"/>
-      <c r="AK25" s="12"/>
-      <c r="AL25" s="12"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="218"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="219"/>
+      <c r="U25" s="183" t="s">
+        <v>47</v>
+      </c>
+      <c r="V25" s="181"/>
+      <c r="W25" s="220"/>
+      <c r="X25" s="181"/>
+      <c r="Y25" s="194"/>
+      <c r="Z25" s="181"/>
+      <c r="AA25" s="181"/>
+      <c r="AB25" s="181"/>
+      <c r="AC25" s="181"/>
+      <c r="AD25" s="181"/>
+      <c r="AE25" s="181"/>
+      <c r="AF25" s="181"/>
+      <c r="AG25" s="181"/>
+      <c r="AH25" s="181"/>
+      <c r="AI25" s="181"/>
+      <c r="AJ25" s="181"/>
+      <c r="AK25" s="47"/>
+      <c r="AL25" s="47"/>
     </row>
     <row r="26" spans="1:39" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="102"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="258"/>
-      <c r="K26" s="259"/>
-      <c r="L26" s="259"/>
-      <c r="M26" s="259"/>
-      <c r="N26" s="259"/>
-      <c r="O26" s="259"/>
-      <c r="P26" s="259"/>
-      <c r="Q26" s="260"/>
-      <c r="R26" s="260"/>
-      <c r="S26" s="260"/>
-      <c r="T26" s="260"/>
-      <c r="U26" s="260"/>
-      <c r="V26" s="12"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="12"/>
-      <c r="AC26" s="12"/>
-      <c r="AD26" s="12"/>
-      <c r="AE26" s="12"/>
-      <c r="AF26" s="12"/>
-      <c r="AG26" s="12"/>
-      <c r="AH26" s="12"/>
-      <c r="AI26" s="12"/>
-      <c r="AJ26" s="12"/>
-      <c r="AK26" s="12"/>
-      <c r="AL26" s="12"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="221"/>
+      <c r="F26" s="222"/>
+      <c r="G26" s="222"/>
+      <c r="H26" s="222"/>
+      <c r="I26" s="223"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="224"/>
+      <c r="R26" s="224"/>
+      <c r="S26" s="224"/>
+      <c r="T26" s="224"/>
+      <c r="U26" s="224"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="225"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="226"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="47"/>
+      <c r="AG26" s="47"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="47"/>
+      <c r="AJ26" s="47"/>
+      <c r="AK26" s="47"/>
+      <c r="AL26" s="47"/>
     </row>
     <row r="27" spans="1:39" ht="28.15" customHeight="1">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="252" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="253"/>
-      <c r="G27" s="253"/>
-      <c r="H27" s="253"/>
-      <c r="I27" s="254"/>
-      <c r="J27" s="255" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27" s="256"/>
-      <c r="L27" s="256"/>
-      <c r="M27" s="256"/>
-      <c r="N27" s="256"/>
-      <c r="O27" s="256"/>
-      <c r="P27" s="256"/>
-      <c r="Q27" s="257" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="227" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="228"/>
+      <c r="G27" s="228"/>
+      <c r="H27" s="228"/>
+      <c r="I27" s="229"/>
+      <c r="J27" s="230" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="231"/>
+      <c r="L27" s="231"/>
+      <c r="M27" s="231"/>
+      <c r="N27" s="231"/>
+      <c r="O27" s="231"/>
+      <c r="P27" s="231"/>
+      <c r="Q27" s="232" t="s">
         <v>6</v>
       </c>
-      <c r="R27" s="257"/>
-      <c r="S27" s="257"/>
-      <c r="T27" s="257"/>
-      <c r="U27" s="257"/>
-      <c r="V27" s="88"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="12"/>
-      <c r="AB27" s="12"/>
-      <c r="AC27" s="12"/>
-      <c r="AD27" s="12"/>
-      <c r="AE27" s="12"/>
-      <c r="AF27" s="12"/>
-      <c r="AG27" s="12"/>
-      <c r="AH27" s="12"/>
-      <c r="AI27" s="12"/>
-      <c r="AJ27" s="12"/>
-      <c r="AK27" s="12"/>
-      <c r="AL27" s="12"/>
+      <c r="R27" s="232"/>
+      <c r="S27" s="232"/>
+      <c r="T27" s="232"/>
+      <c r="U27" s="232"/>
+      <c r="V27" s="233"/>
+      <c r="W27" s="225"/>
+      <c r="X27" s="226"/>
+      <c r="Y27" s="226"/>
+      <c r="Z27" s="47"/>
+      <c r="AA27" s="47"/>
+      <c r="AB27" s="47"/>
+      <c r="AC27" s="47"/>
+      <c r="AD27" s="47"/>
+      <c r="AE27" s="47"/>
+      <c r="AF27" s="47"/>
+      <c r="AG27" s="47"/>
+      <c r="AH27" s="47"/>
+      <c r="AI27" s="47"/>
+      <c r="AJ27" s="47"/>
+      <c r="AK27" s="47"/>
+      <c r="AL27" s="47"/>
     </row>
     <row r="28" spans="1:39" ht="11.25" customHeight="1">
-      <c r="X28" s="64"/>
-      <c r="Y28" s="89"/>
-      <c r="Z28" s="89"/>
-      <c r="AA28" s="89"/>
-      <c r="AB28" s="89"/>
-      <c r="AC28" s="89"/>
-      <c r="AD28" s="89"/>
-      <c r="AE28" s="55"/>
-      <c r="AF28" s="55"/>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="52"/>
-      <c r="AK28" s="53"/>
+      <c r="X28" s="234"/>
+      <c r="Y28" s="235"/>
+      <c r="Z28" s="235"/>
+      <c r="AA28" s="235"/>
+      <c r="AB28" s="235"/>
+      <c r="AC28" s="235"/>
+      <c r="AD28" s="235"/>
+      <c r="AE28" s="236"/>
+      <c r="AF28" s="236"/>
+      <c r="AG28" s="237"/>
+      <c r="AH28" s="237"/>
+      <c r="AI28" s="237"/>
+      <c r="AJ28" s="238"/>
+      <c r="AK28" s="239"/>
     </row>
     <row r="29" spans="1:39">
-      <c r="R29" s="1" t="s">
+      <c r="R29" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="X29" s="64"/>
-      <c r="Y29" s="55"/>
-      <c r="Z29" s="55"/>
-      <c r="AA29" s="55"/>
-      <c r="AB29" s="55"/>
-      <c r="AC29" s="55"/>
-      <c r="AD29" s="55"/>
-      <c r="AE29" s="55"/>
-      <c r="AF29" s="55"/>
-      <c r="AG29" s="51"/>
-      <c r="AH29" s="51"/>
-      <c r="AI29" s="51"/>
-      <c r="AJ29" s="52"/>
-      <c r="AK29" s="53"/>
+      <c r="X29" s="234"/>
+      <c r="Y29" s="236"/>
+      <c r="Z29" s="236"/>
+      <c r="AA29" s="236"/>
+      <c r="AB29" s="236"/>
+      <c r="AC29" s="236"/>
+      <c r="AD29" s="236"/>
+      <c r="AE29" s="236"/>
+      <c r="AF29" s="236"/>
+      <c r="AG29" s="237"/>
+      <c r="AH29" s="237"/>
+      <c r="AI29" s="237"/>
+      <c r="AJ29" s="238"/>
+      <c r="AK29" s="239"/>
     </row>
     <row r="30" spans="1:39">
-      <c r="X30" s="64"/>
-      <c r="Y30" s="55"/>
-      <c r="Z30" s="55"/>
-      <c r="AA30" s="55"/>
-      <c r="AB30" s="55"/>
-      <c r="AC30" s="55"/>
-      <c r="AD30" s="55"/>
-      <c r="AE30" s="55"/>
-      <c r="AF30" s="55"/>
-      <c r="AG30" s="54"/>
-      <c r="AH30" s="54"/>
-      <c r="AI30" s="54"/>
-      <c r="AJ30" s="52"/>
-      <c r="AK30" s="53"/>
+      <c r="X30" s="234"/>
+      <c r="Y30" s="236"/>
+      <c r="Z30" s="236"/>
+      <c r="AA30" s="236"/>
+      <c r="AB30" s="236"/>
+      <c r="AC30" s="236"/>
+      <c r="AD30" s="236"/>
+      <c r="AE30" s="236"/>
+      <c r="AF30" s="236"/>
+      <c r="AG30" s="240"/>
+      <c r="AH30" s="240"/>
+      <c r="AI30" s="240"/>
+      <c r="AJ30" s="238"/>
+      <c r="AK30" s="239"/>
     </row>
     <row r="31" spans="1:39">
-      <c r="W31" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="X31" s="91"/>
-      <c r="Y31" s="91"/>
-      <c r="Z31" s="91"/>
-      <c r="AA31" s="91"/>
-      <c r="AB31" s="92"/>
-      <c r="AD31" s="64"/>
-      <c r="AE31" s="65"/>
-      <c r="AF31" s="65"/>
-      <c r="AG31" s="63"/>
-      <c r="AH31" s="63"/>
-      <c r="AI31" s="63"/>
-      <c r="AJ31" s="54"/>
-      <c r="AK31" s="54"/>
+      <c r="W31" s="241" t="s">
+        <v>49</v>
+      </c>
+      <c r="X31" s="242"/>
+      <c r="Y31" s="242"/>
+      <c r="Z31" s="242"/>
+      <c r="AA31" s="242"/>
+      <c r="AB31" s="243"/>
+      <c r="AD31" s="234"/>
+      <c r="AE31" s="236"/>
+      <c r="AF31" s="236"/>
+      <c r="AG31" s="240"/>
+      <c r="AH31" s="240"/>
+      <c r="AI31" s="240"/>
+      <c r="AJ31" s="240"/>
+      <c r="AK31" s="240"/>
     </row>
     <row r="32" spans="1:39">
-      <c r="W32" s="93" t="s">
-        <v>49</v>
-      </c>
-      <c r="X32" s="94"/>
-      <c r="Y32" s="94"/>
-      <c r="Z32" s="94"/>
-      <c r="AA32" s="94"/>
-      <c r="AB32" s="94"/>
-      <c r="AC32" s="94"/>
-      <c r="AD32" s="94"/>
-      <c r="AE32" s="94"/>
-      <c r="AF32" s="94"/>
-      <c r="AG32" s="94"/>
-      <c r="AH32" s="94"/>
-      <c r="AI32" s="94"/>
-      <c r="AJ32" s="95"/>
-      <c r="AK32" s="96"/>
+      <c r="W32" s="244" t="s">
+        <v>48</v>
+      </c>
+      <c r="X32" s="245"/>
+      <c r="Y32" s="245"/>
+      <c r="Z32" s="245"/>
+      <c r="AA32" s="245"/>
+      <c r="AB32" s="245"/>
+      <c r="AC32" s="245"/>
+      <c r="AD32" s="245"/>
+      <c r="AE32" s="245"/>
+      <c r="AF32" s="245"/>
+      <c r="AG32" s="245"/>
+      <c r="AH32" s="245"/>
+      <c r="AI32" s="245"/>
+      <c r="AJ32" s="242"/>
+      <c r="AK32" s="243"/>
     </row>
     <row r="33" spans="23:37">
-      <c r="W33" s="66"/>
-      <c r="X33" s="64"/>
-      <c r="Y33" s="97"/>
-      <c r="Z33" s="97"/>
-      <c r="AA33" s="97"/>
-      <c r="AB33" s="97"/>
-      <c r="AC33" s="97"/>
-      <c r="AD33" s="97"/>
-      <c r="AE33" s="97"/>
-      <c r="AF33" s="97"/>
-      <c r="AG33" s="97"/>
-      <c r="AH33" s="97"/>
-      <c r="AI33" s="97"/>
-      <c r="AJ33" s="97" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK33" s="98"/>
+      <c r="W33" s="246"/>
+      <c r="X33" s="234"/>
+      <c r="Y33" s="247"/>
+      <c r="Z33" s="247"/>
+      <c r="AA33" s="247"/>
+      <c r="AB33" s="247"/>
+      <c r="AC33" s="247"/>
+      <c r="AD33" s="247"/>
+      <c r="AE33" s="247"/>
+      <c r="AF33" s="247"/>
+      <c r="AG33" s="247"/>
+      <c r="AH33" s="247"/>
+      <c r="AI33" s="247"/>
+      <c r="AJ33" s="247" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK33" s="248"/>
     </row>
     <row r="34" spans="23:37">
-      <c r="W34" s="66"/>
-      <c r="X34" s="64"/>
-      <c r="Y34" s="97"/>
-      <c r="Z34" s="97"/>
-      <c r="AA34" s="97"/>
-      <c r="AB34" s="97"/>
-      <c r="AC34" s="97"/>
-      <c r="AD34" s="97"/>
-      <c r="AE34" s="97"/>
-      <c r="AF34" s="97"/>
-      <c r="AG34" s="97"/>
-      <c r="AH34" s="97"/>
-      <c r="AI34" s="97"/>
-      <c r="AJ34" s="97"/>
-      <c r="AK34" s="98"/>
+      <c r="W34" s="246"/>
+      <c r="X34" s="234"/>
+      <c r="Y34" s="247"/>
+      <c r="Z34" s="247"/>
+      <c r="AA34" s="247"/>
+      <c r="AB34" s="247"/>
+      <c r="AC34" s="247"/>
+      <c r="AD34" s="247"/>
+      <c r="AE34" s="247"/>
+      <c r="AF34" s="247"/>
+      <c r="AG34" s="247"/>
+      <c r="AH34" s="247"/>
+      <c r="AI34" s="247"/>
+      <c r="AJ34" s="247"/>
+      <c r="AK34" s="248"/>
     </row>
     <row r="35" spans="23:37">
-      <c r="W35" s="67"/>
-      <c r="X35" s="68"/>
-      <c r="Y35" s="99"/>
-      <c r="Z35" s="99"/>
-      <c r="AA35" s="99"/>
-      <c r="AB35" s="99"/>
-      <c r="AC35" s="99"/>
-      <c r="AD35" s="99"/>
-      <c r="AE35" s="99"/>
-      <c r="AF35" s="99"/>
-      <c r="AG35" s="99"/>
-      <c r="AH35" s="99"/>
-      <c r="AI35" s="99"/>
-      <c r="AJ35" s="99"/>
-      <c r="AK35" s="100"/>
+      <c r="W35" s="249"/>
+      <c r="X35" s="250"/>
+      <c r="Y35" s="251"/>
+      <c r="Z35" s="251"/>
+      <c r="AA35" s="251"/>
+      <c r="AB35" s="251"/>
+      <c r="AC35" s="251"/>
+      <c r="AD35" s="251"/>
+      <c r="AE35" s="251"/>
+      <c r="AF35" s="251"/>
+      <c r="AG35" s="251"/>
+      <c r="AH35" s="251"/>
+      <c r="AI35" s="251"/>
+      <c r="AJ35" s="251"/>
+      <c r="AK35" s="252"/>
     </row>
     <row r="37" spans="23:37" ht="84.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="Y28:AD28"/>
+    <mergeCell ref="W31:AB31"/>
+    <mergeCell ref="W32:AI32"/>
+    <mergeCell ref="AJ32:AK35"/>
+    <mergeCell ref="Y33:AI35"/>
+    <mergeCell ref="D8:D27"/>
+    <mergeCell ref="C8:C27"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="M5:U6"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="U16:Y16"/>
+    <mergeCell ref="AL5:AL6"/>
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AB5:AD6"/>
+    <mergeCell ref="AE5:AG6"/>
+    <mergeCell ref="AH5:AJ6"/>
+    <mergeCell ref="Y5:AA6"/>
+    <mergeCell ref="AH8:AI8"/>
+    <mergeCell ref="Z8:AG10"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="K8:M10"/>
+    <mergeCell ref="N8:Y10"/>
+    <mergeCell ref="E8:J10"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH3:AJ4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="Q12:Q15"/>
+    <mergeCell ref="Y12:Y15"/>
+    <mergeCell ref="T12:T15"/>
+    <mergeCell ref="R12:R15"/>
+    <mergeCell ref="Q16:T19"/>
+    <mergeCell ref="S12:S15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="P12:P15"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="K11:M15"/>
+    <mergeCell ref="AC12:AC15"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="AH21:AI21"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="AG16:AG19"/>
+    <mergeCell ref="U12:U15"/>
+    <mergeCell ref="V12:V15"/>
+    <mergeCell ref="W12:W15"/>
+    <mergeCell ref="X12:X15"/>
+    <mergeCell ref="AB12:AB15"/>
+    <mergeCell ref="AE12:AE15"/>
+    <mergeCell ref="Z17:AC19"/>
+    <mergeCell ref="U17:Y19"/>
+    <mergeCell ref="Z11:AA15"/>
     <mergeCell ref="J21:S21"/>
     <mergeCell ref="K23:T23"/>
     <mergeCell ref="K24:T24"/>
@@ -5667,76 +5605,13 @@
     <mergeCell ref="AG12:AG15"/>
     <mergeCell ref="AF12:AF15"/>
     <mergeCell ref="M18:P18"/>
-    <mergeCell ref="AC12:AC15"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="AH21:AI21"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="AG16:AG19"/>
-    <mergeCell ref="U12:U15"/>
-    <mergeCell ref="V12:V15"/>
-    <mergeCell ref="W12:W15"/>
-    <mergeCell ref="X12:X15"/>
-    <mergeCell ref="AB12:AB15"/>
-    <mergeCell ref="AE12:AE15"/>
-    <mergeCell ref="Z17:AC19"/>
-    <mergeCell ref="U17:Y19"/>
-    <mergeCell ref="Z11:AA15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="P12:P15"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="K11:M15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="Q12:Q15"/>
-    <mergeCell ref="Y12:Y15"/>
-    <mergeCell ref="T12:T15"/>
-    <mergeCell ref="R12:R15"/>
-    <mergeCell ref="Q16:T19"/>
-    <mergeCell ref="S12:S15"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH3:AJ4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="Y5:AA6"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="Z8:AG10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="K8:M10"/>
-    <mergeCell ref="N8:Y10"/>
-    <mergeCell ref="E8:J10"/>
-    <mergeCell ref="AL5:AL6"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="AB5:AD6"/>
-    <mergeCell ref="AE5:AG6"/>
-    <mergeCell ref="AH5:AJ6"/>
-    <mergeCell ref="D8:D27"/>
-    <mergeCell ref="C8:C27"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="M5:U6"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="U16:Y16"/>
-    <mergeCell ref="Y28:AD28"/>
-    <mergeCell ref="W31:AB31"/>
-    <mergeCell ref="W32:AI32"/>
-    <mergeCell ref="AJ32:AK35"/>
-    <mergeCell ref="Y33:AI35"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="J22:L22"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>